<commit_message>
final code for generating skelton code
</commit_message>
<xml_diff>
--- a/SoftwareDesignUsingNLP/data/Healthcare Data/output.xlsx
+++ b/SoftwareDesignUsingNLP/data/Healthcare Data/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>User</t>
   </si>
@@ -38,7 +38,7 @@
     <t>['Recruit Doctors'],['Offer Plan']</t>
   </si>
   <si>
-    <t>{'Policy_number', 'Acc_type', 'Doctor_Name', 'Hospital_Address', 'Patient_Name'},{'Preventive_care', 'Policy_coverage_details', 'Patient_Address', 'List_plan'}</t>
+    <t>{'doctor_licence_number', 'Doctor_Name', 'hospital_department'},{'List_plan', 'Name_of_clinics', 'Preventive_care'}</t>
   </si>
   <si>
     <t xml:space="preserve"> plan the stay, shift their care to outpatient clinics</t>
@@ -47,7 +47,7 @@
     <t>['Offer Plan', 'Patient Admission'],['Patient Transfer']</t>
   </si>
   <si>
-    <t>{'Preventive_care', 'Policy_coverage_details', 'Patient_Address', 'List_plan'}{'Policy_number', 'Patient_prior_condition', 'Patient_age', 'Patient_Name', 'Coverage_policy'},{'Policy_number', 'Acc_type', 'Doctor_Name', 'Hospital_Address', 'Patient_Name'}</t>
+    <t>{'List_plan', 'Name_of_clinics', 'Preventive_care'}{'Patient_age', 'Schedule_time', 'Name_of_clinics', 'Customer_phone'},{'Preventive_care', 'Address_Of_clinics', 'Policy_number'}</t>
   </si>
   <si>
     <t xml:space="preserve"> emphasize more on preventive care to my patients</t>
@@ -56,7 +56,7 @@
     <t>['Provide reccommendation']</t>
   </si>
   <si>
-    <t>{'Policy_number', 'Acc_type', 'Doctor_Name', 'Hospital_Address', 'Patient_Name'}</t>
+    <t>{'Acc_type', 'Address_Of_clinics', 'Hospital_Address', 'Preventive_care'}</t>
   </si>
   <si>
     <t xml:space="preserve"> employ salaried doctors, paid per service</t>
@@ -65,7 +65,7 @@
     <t>['Recruit Doctors', 'Recruit Visiting Doctors'],['Contact doctor']</t>
   </si>
   <si>
-    <t>{'Policy_number', 'Acc_type', 'Doctor_Name', 'Hospital_Address', 'Patient_Name'}{'Policy_number', 'Acc_type', 'Doctor_Name', 'Hospital_Address', 'Patient_Name'},{'Patient_prior_condition', 'hospital_department', 'Doctor_Name', 'Customer_phone', 'Coverage_policy'}</t>
+    <t>{'doctor_licence_number', 'Doctor_Name', 'hospital_department'}{'doctor_licence_number', 'Coverage_policy', 'Doctor_Name', 'Hourly_charge_doctor', 'hospital_department'},{'Customer_phone', 'Doctor_Name', 'Hospital_Address', 'Patient_prior_condition', 'Patient_age'}</t>
   </si>
   <si>
     <t>Health Plan Member</t>
@@ -77,7 +77,7 @@
     <t>['Offer Plan']</t>
   </si>
   <si>
-    <t>{'Preventive_care', 'Policy_coverage_details', 'Patient_Address', 'List_plan'}</t>
+    <t>{'List_plan', 'Name_of_clinics', 'Preventive_care'}</t>
   </si>
   <si>
     <t xml:space="preserve"> find nearby doctors and hospitals</t>
@@ -86,7 +86,7 @@
     <t>['List of hospitals under plan', 'Contact doctor']</t>
   </si>
   <si>
-    <t>{'Schedule_time', 'Address_Of_clinics', 'X,Y_Coordinates', 'Hospital_Address', 'List_plan'}{'Patient_prior_condition', 'hospital_department', 'Doctor_Name', 'Customer_phone', 'Coverage_policy'}</t>
+    <t>{'X,Y_Coordinates'}{'Customer_phone', 'Doctor_Name', 'Hospital_Address', 'Patient_prior_condition', 'Patient_age'}</t>
   </si>
   <si>
     <t>Patient</t>
@@ -98,7 +98,7 @@
     <t>['Payment Process ']</t>
   </si>
   <si>
-    <t>{'Policy_number', 'Discharge_amount', 'Patient_age', 'Acc_type', 'Patient_Name'}</t>
+    <t>{'Acc_type', 'Schedule_time', 'Doctor_Name', 'Hospital_Address', 'Discharge_amount'}</t>
   </si>
   <si>
     <t xml:space="preserve"> see my medical reports online</t>
@@ -107,13 +107,16 @@
     <t>['Schedule visit']</t>
   </si>
   <si>
+    <t>{'Schedule_time', 'Doctor_available_time'}</t>
+  </si>
+  <si>
     <t xml:space="preserve"> see my Doctor, schedule my visit online</t>
   </si>
   <si>
     <t>['Schedule visit', 'Recruit Doctors'],['Recruit Visiting Doctors', 'Schedule visit']</t>
   </si>
   <si>
-    <t>{'Policy_number', 'Acc_type', 'Doctor_Name', 'Hospital_Address', 'Patient_Name'}{'Policy_number', 'Acc_type', 'Doctor_Name', 'Hospital_Address', 'Patient_Name'},{'Policy_number', 'Acc_type', 'Doctor_Name', 'Hospital_Address', 'Patient_Name'}{'Policy_number', 'Acc_type', 'Doctor_Name', 'Hospital_Address', 'Patient_Name'}</t>
+    <t>{'Schedule_time', 'Doctor_available_time'}{'doctor_licence_number', 'Doctor_Name', 'hospital_department'},{'doctor_licence_number', 'Coverage_policy', 'Doctor_Name', 'Hourly_charge_doctor', 'hospital_department'}{'Schedule_time', 'Doctor_available_time'}</t>
   </si>
 </sst>
 </file>
@@ -593,7 +596,7 @@
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -601,13 +604,13 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>